<commit_message>
Update Min Area Schedule
</commit_message>
<xml_diff>
--- a/pyHP.tab/Residential.panel/Minimal Area Req.pushbutton/Minimal area requirement.xlsx
+++ b/pyHP.tab/Residential.panel/Minimal Area Req.pushbutton/Minimal area requirement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Shared\Archilizer\Clients\Hutchinson &amp; Partners\5_Computation\pyChilizer\Minimal area req\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daria Ivanciucova\Documents\GitHub\pyHP\pyHP.tab\Residential.panel\Minimal Area Req.pushbutton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78205BE0-7227-4C58-8EB8-8E94203B302B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547C200D-09B4-4C0D-82D4-769673065105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Bedroom 1</t>
-  </si>
-  <si>
-    <t>Bedroom 2</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Bedroom 3</t>
-  </si>
-  <si>
     <t>1B2P</t>
   </si>
   <si>
@@ -60,16 +48,28 @@
     <t>4B6P</t>
   </si>
   <si>
-    <t>Living / Dining / Kitchen</t>
-  </si>
-  <si>
     <t>GIA</t>
   </si>
   <si>
-    <t>Bedroom 4</t>
-  </si>
-  <si>
-    <t>Bedroom</t>
+    <t>BEDROOM</t>
+  </si>
+  <si>
+    <t>BEDROOM 1</t>
+  </si>
+  <si>
+    <t>BEDROOM 2</t>
+  </si>
+  <si>
+    <t>BEDROOM 3</t>
+  </si>
+  <si>
+    <t>BEDROOM 4</t>
+  </si>
+  <si>
+    <t>STORAGE</t>
+  </si>
+  <si>
+    <t>LIVING / DINING / KITCHEN</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,30 +440,30 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>37</v>
@@ -672,5 +672,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>